<commit_message>
grap the first EPW file... not just the first file
</commit_message>
<xml_diff>
--- a/spec/files/0_3_0_outputs.xlsx
+++ b/spec/files/0_3_0_outputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="9640" yWindow="7780" windowWidth="25600" windowHeight="16060" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2491,13 +2491,13 @@
     <t>../../spec/files/small_seed.osm</t>
   </si>
   <si>
-    <t>../../spec/files/*.epw</t>
-  </si>
-  <si>
     <t>0_3_0_outputs</t>
   </si>
   <si>
     <t>OSM</t>
+  </si>
+  <si>
+    <t>../../spec/files/*</t>
   </si>
 </sst>
 </file>
@@ -6573,8 +6573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7014,7 +7014,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28">
@@ -7039,10 +7039,10 @@
         <v>32</v>
       </c>
       <c r="B40" s="30" t="s">
+        <v>816</v>
+      </c>
+      <c r="C40" s="30" t="s">
         <v>817</v>
-      </c>
-      <c r="C40" s="30" t="s">
-        <v>818</v>
       </c>
       <c r="D40" s="54" t="s">
         <v>815</v>

</xml_diff>

<commit_message>
error out if measure cannot be found. cleanup all tests
</commit_message>
<xml_diff>
--- a/spec/files/0_3_0_outputs.xlsx
+++ b/spec/files/0_3_0_outputs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="7780" windowWidth="25600" windowHeight="16060" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="9640" yWindow="7780" windowWidth="25600" windowHeight="16060" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2413" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="819">
   <si>
     <t>type</t>
   </si>
@@ -6573,7 +6573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -7096,9 +7096,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7264,6 +7264,9 @@
       </c>
       <c r="B4" s="40" t="s">
         <v>74</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>267</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>75</v>

</xml_diff>